<commit_message>
Updates Data and maps.
</commit_message>
<xml_diff>
--- a/data/FINAL alternative_trails_data.xlsx
+++ b/data/FINAL alternative_trails_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25616"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carloscamara/Documents/Git repos/alternative_trails_map/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livewarwickac-my.sharepoint.com/personal/u2056714_live_warwick_ac_uk/Documents/WARWICK All Other Work/Alternative Trails Cov City of Culture/Alternative Trails Map_AllData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799548D6-AE1F-534E-8A7A-70E7FFAE1F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="8_{6378A6F4-8F89-417B-8868-5359B07D23DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAE7DD69-C12D-49F4-8178-082959C417B4}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10560" tabRatio="499" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="499" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="alternative_trails_data" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="107">
   <si>
     <t>name</t>
   </si>
@@ -350,6 +350,12 @@
     <t>KOCO2.JPG</t>
   </si>
   <si>
+    <t>V_KOCO.mp3</t>
+  </si>
+  <si>
+    <t>The KOCO building provided the space for training men and women under many different projects. The Coventry Cooperative Agency worked from here. They also provided the space for projects training the unemployed, and for anti-racism meetings in Coventry. Training for workers based in different organisations also took place here.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Frank Walsh House </t>
   </si>
   <si>
@@ -365,6 +371,12 @@
     <t>FWALSH2.JPG</t>
   </si>
   <si>
+    <t>P_FWHouse.mp3</t>
+  </si>
+  <si>
+    <t>Frank Walsh House provided supported living to the elderly and was one of the first Asian sheltered living spaces in Coventry. They hosted the Asian Women's and Men's Groups a. The space has changed drastically over the years.  Panahghar held a lot of its support group meetings at Franks Walsh House. The women remember this spot fondly; they started their trip to Glasgow from this point (For more on this, see St Paul's Community Centre on the map). Location was also key to the importance of Frank Walsh House as a meeting place; it was close to temples, gurudwaras, and mosques, and thus served as a focal point for the community.</t>
+  </si>
+  <si>
     <t xml:space="preserve"> St. Barnabus Church and Family Centre</t>
   </si>
   <si>
@@ -377,12 +389,21 @@
     <t>barnabus2.JPG</t>
   </si>
   <si>
+    <t>V_Barnabus.mp3</t>
+  </si>
+  <si>
+    <t>The St. Barnabus Church and Family Centre served as one of the first Asian daycare centres. They held daycare activities for the elderly, and on Tuesdays, for elderly Asians. The centre provided space for group meetings, armchair exercises, personal care, and board games, helping community members build connections and stay active. The other side of the building also hosted youth groups and children's playgroups. Reflective of the surge, in the 1980s, in both national and social services support for community-based initiatives in the UK, this was a thriving centre at that time.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Elm Bank </t>
   </si>
   <si>
     <t>Mile Ln,  CV1 2LQ</t>
   </si>
   <si>
+    <t>Elm Bank was initially a Teacher Training centre and later became a Training centre. Rooms were hired out for training including to Asian women’s organisations which did courses such as computer skills, project Management skills, and Team Building etc. Such training enabled voluntary organisations across the city to connect and network with each other.</t>
+  </si>
+  <si>
     <t>St. Peters Church, Hillfields</t>
   </si>
   <si>
@@ -405,6 +426,11 @@
   </si>
   <si>
     <t>stpauls2.JPG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St. Paul’s church became instrumental in exploring community development in partnership with local authority by taking responsibility to offer assistance in programs delivery. The groups meeting at church were often used to receive the information on home working projects. The Shanti Bhavan ladies group, now known as Ekta Unity, met here every Monday in one of the small rooms attached to St Paul’s church. The group was able to use the kitchen and was given storage facilities. At the time when Foleshill Women Training project was looking for premises to start the catering enterprise, the vicar of St Paul’s was very active local church partnerships to offer support to management committee members. The community was engaged by holding events to provide information on services available on health and voluntary and statutory services. Women were provided with advice on social benefits, education and work. These were predominately attended by Asian women. Voluntary groups also were encouraged to use the centre as there was an overlap with the services and the people attending.
+The Community Mental Health team started support groups and care groups for women and men in here. The advantage of using the venue was that it was not a medical facility and people could go there without any label or stigma attached. It was a safe space for many. The NHS Partnership Trust workers using the church faced some challenges about the Asian community using church premises, as well as equal access to the space by men and women. However, they succeeded in navigating these issues in a culturally sensitive way, and the numbers in attendance kept growing. 
+</t>
   </si>
   <si>
     <t>Berry St (the 1st Panagarh Adminstrative Office)</t>
@@ -489,24 +515,6 @@
   </si>
   <si>
     <t>ALTERNATIVE TRAILS : Mapping South Asian Women’s Activism</t>
-  </si>
-  <si>
-    <t>groupphotowebsite.jpeg</t>
-  </si>
-  <si>
-    <t>V_audio1.mp4</t>
-  </si>
-  <si>
-    <t>P_audio1.mp4</t>
-  </si>
-  <si>
-    <t>I_audio1.ogg</t>
-  </si>
-  <si>
-    <t>I_audio2.ogg</t>
-  </si>
-  <si>
-    <t>JT_audio1.mp3</t>
   </si>
   <si>
     <r>
@@ -540,6 +548,43 @@
   <si>
     <r>
       <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>The word 'activism'</t>
+    </r>
+  </si>
+  <si>
+    <t>groupphotowebsite.jpeg</t>
+  </si>
+  <si>
+    <t>V_audio1.mp4</t>
+  </si>
+  <si>
+    <t>P_audio1.mp4</t>
+  </si>
+  <si>
+    <t>I_audio1.ogg</t>
+  </si>
+  <si>
+    <t>I_audio2.ogg</t>
+  </si>
+  <si>
+    <t>JT_audio1.mp3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <b/>
         <sz val="12"/>
         <color theme="1"/>
@@ -600,31 +645,12 @@
 ‘I think it's because the funding is set up in such a way, sort of set up to divide and rule. But the organisations that realised that started networking, partnering, and putting in bids together, setting up steering groups and all that’. </t>
     </r>
   </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> bottom of the map titled </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"The word 'activism'" </t>
-    </r>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -796,12 +822,21 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b/>
-      <sz val="10"/>
-      <color theme="1"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="35">
@@ -1194,23 +1229,21 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1570,20 +1603,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20:E20"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" style="1" customWidth="1"/>
-    <col min="3" max="13" width="10.83203125" style="1"/>
-    <col min="14" max="14" width="54.5" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="18.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.875" style="1" customWidth="1"/>
+    <col min="3" max="13" width="10.875" style="1"/>
+    <col min="14" max="14" width="54.625" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1627,7 +1660,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="46.5">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -1665,7 +1698,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="55.5" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -1701,7 +1734,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="39.950000000000003" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
@@ -1737,7 +1770,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="46.5">
       <c r="A5" s="3" t="s">
         <v>37</v>
       </c>
@@ -1773,7 +1806,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="39.6" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>44</v>
       </c>
@@ -1801,7 +1834,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="50.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="50.45" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>47</v>
       </c>
@@ -1833,7 +1866,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1849,7 +1882,7 @@
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
     </row>
-    <row r="9" spans="1:14" ht="60" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="52.5">
       <c r="A9" s="3" t="s">
         <v>52</v>
       </c>
@@ -1874,22 +1907,26 @@
       <c r="H9" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-    </row>
-    <row r="10" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+      <c r="I9" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="39.6">
       <c r="A10" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D10">
         <v>52.416781666470399</v>
@@ -1899,27 +1936,31 @@
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="39.6">
+      <c r="A11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-    </row>
-    <row r="11" spans="1:14" ht="45" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D11">
         <v>52.4232904047688</v>
@@ -1929,27 +1970,31 @@
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-    </row>
-    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="26.45">
       <c r="A12" s="3" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D12">
         <v>52.400678947082902</v>
@@ -1960,22 +2005,24 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-    </row>
-    <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.2">
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="26.45">
       <c r="A13" s="3" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="D13">
         <v>52.412871241874498</v>
@@ -1984,10 +2031,10 @@
         <v>-1.5015381884318699</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
@@ -1997,15 +2044,15 @@
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
     </row>
-    <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="27">
       <c r="A14" s="3" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="D14">
         <v>52.427035607113801</v>
@@ -2015,27 +2062,29 @@
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-    </row>
-    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="39.6">
       <c r="A15" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D15">
         <v>52.412944006938098</v>
@@ -2053,15 +2102,15 @@
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
     </row>
-    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="26.45">
       <c r="A16" s="3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D16">
         <v>52.422362708072697</v>
@@ -2071,31 +2120,31 @@
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="60" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="52.5">
       <c r="A17" s="3" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="D17">
         <v>52.439421466671902</v>
@@ -2107,17 +2156,17 @@
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
       <c r="N17" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -2133,14 +2182,14 @@
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
     </row>
-    <row r="19" spans="1:14" ht="45" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
+    <row r="19" spans="1:14" ht="39">
+      <c r="A19" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
@@ -2150,48 +2199,42 @@
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="51" x14ac:dyDescent="0.2">
-      <c r="A20" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B20" s="16" t="s">
+    </row>
+    <row r="20" spans="1:14" ht="48.75">
+      <c r="A20" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="4">
-        <v>52.381</v>
-      </c>
-      <c r="E20" s="4">
-        <v>-1.5649999999999999</v>
-      </c>
-      <c r="F20" s="17"/>
-      <c r="G20" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="J20" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="K20" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="L20" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="M20" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="N20" s="17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="N20" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -2207,7 +2250,7 @@
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2223,7 +2266,7 @@
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -2239,7 +2282,7 @@
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -2255,7 +2298,7 @@
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -2271,7 +2314,7 @@
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2287,7 +2330,7 @@
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2303,175 +2346,175 @@
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>

</xml_diff>